<commit_message>
OutLier Statistics, And Updated Resources
</commit_message>
<xml_diff>
--- a/Resources/resources.xlsx
+++ b/Resources/resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roumo\Desktop\WaterLevel\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DC319E-C980-4D9C-BA2C-29FC859708EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE7983E-F04A-4CC9-A930-1BA58F1464E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -611,7 +611,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>